<commit_message>
deuxieme matrice RACI General
</commit_message>
<xml_diff>
--- a/Documents/Matrice RACI Reseau/Matrice_RACI_Reseau.xlsx
+++ b/Documents/Matrice RACI Reseau/Matrice_RACI_Reseau.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azn_j\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azn_j\Desktop\ESGI\2017-2018\Projet_annuel\Projet_Annuel2i\Documents\Matrice RACI Reseau\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>RACI Chart (Roles and Responsibilities Matrix)</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>,,,,</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>AR</t>
   </si>
 </sst>
 </file>
@@ -668,6 +674,34 @@
     <xf numFmtId="14" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -686,6 +720,9 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -753,37 +790,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1168,7 +1174,7 @@
   <dimension ref="B1:I23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,23 +1220,23 @@
         <v>24</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="45"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="55"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="48"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="58"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="2:9" ht="7.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1276,23 +1282,23 @@
         <v>27</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="50"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="61"/>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="2:9" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="53"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="64"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1306,7 +1312,7 @@
       <c r="I12" s="3"/>
     </row>
     <row r="14" spans="2:9" ht="25.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="43" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="10" t="s">
@@ -1322,28 +1328,28 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="2:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="51" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="32"/>
-      <c r="D15" s="74" t="s">
-        <v>23</v>
+      <c r="D15" s="44" t="s">
+        <v>39</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G15" s="30"/>
       <c r="H15" s="31"/>
     </row>
     <row r="16" spans="2:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="82" t="s">
+      <c r="B16" s="52" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="6"/>
-      <c r="D16" s="75" t="s">
+      <c r="D16" s="45" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="7" t="s">
@@ -1356,31 +1362,31 @@
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="51" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="32"/>
-      <c r="D17" s="76" t="s">
+      <c r="D17" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="78" t="s">
+      <c r="E17" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="78" t="s">
+      <c r="F17" s="48" t="s">
         <v>23</v>
       </c>
       <c r="G17" s="33"/>
       <c r="H17" s="34"/>
     </row>
     <row r="18" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="82" t="s">
+      <c r="B18" s="52" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="6"/>
-      <c r="D18" s="75" t="s">
+      <c r="D18" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="79" t="s">
+      <c r="E18" s="49" t="s">
         <v>23</v>
       </c>
       <c r="F18" s="7" t="s">
@@ -1390,51 +1396,49 @@
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="2:8" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="81" t="s">
-        <v>37</v>
-      </c>
+      <c r="B19" s="51"/>
       <c r="C19" s="32"/>
-      <c r="D19" s="77" t="s">
+      <c r="D19" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="80" t="s">
+      <c r="E19" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="80" t="s">
+      <c r="F19" s="50" t="s">
         <v>23</v>
       </c>
       <c r="G19" s="35"/>
       <c r="H19" s="36"/>
     </row>
     <row r="20" spans="2:8" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="82" t="s">
+      <c r="B20" s="52" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="6"/>
-      <c r="D20" s="75" t="s">
+      <c r="D20" s="45" t="s">
         <v>23</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="79" t="s">
+      <c r="F20" s="49" t="s">
         <v>23</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="2:8" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="81" t="s">
+      <c r="B21" s="51" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="32"/>
-      <c r="D21" s="77" t="s">
+      <c r="D21" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="80" t="s">
+      <c r="E21" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="80" t="s">
+      <c r="F21" s="50" t="s">
         <v>23</v>
       </c>
       <c r="G21" s="37"/>
@@ -1442,13 +1446,13 @@
     </row>
     <row r="22" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="54" t="s">
+      <c r="D23" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="56"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1516,23 +1520,23 @@
         <v>9</v>
       </c>
       <c r="C5" s="14"/>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="62"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="73"/>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="65"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="76"/>
       <c r="I6" s="14"/>
     </row>
     <row r="7" spans="2:9" ht="7.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1578,23 +1582,23 @@
         <v>14</v>
       </c>
       <c r="C10" s="14"/>
-      <c r="D10" s="66" t="s">
+      <c r="D10" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="68"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="79"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="71"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="82"/>
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -1692,13 +1696,13 @@
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="57" t="s">
+      <c r="D22" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="58"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="59"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="70"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H24" s="11" t="s">

</xml_diff>

<commit_message>
Push apres entrevue avec le prof reseau
Plus de detail dans le schema packet tracer et plus de fonction dans la matrice RACI Reseau
</commit_message>
<xml_diff>
--- a/Documents/Matrice RACI Reseau/Matrice_RACI_Reseau.xlsx
+++ b/Documents/Matrice RACI Reseau/Matrice_RACI_Reseau.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="64">
   <si>
     <t>RACI Chart (Roles and Responsibilities Matrix)</t>
   </si>
@@ -197,10 +197,31 @@
     <t>RECETTE</t>
   </si>
   <si>
-    <t>Cout du service</t>
-  </si>
-  <si>
-    <t>Benefice etc..</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Entrevu avec client et validation</t>
+  </si>
+  <si>
+    <t>Configuration des interfaces</t>
+  </si>
+  <si>
+    <t>Configuration Ipsec</t>
+  </si>
+  <si>
+    <t>Routage</t>
+  </si>
+  <si>
+    <t>Choix du Sous traitant</t>
+  </si>
+  <si>
+    <t>Validation mise en place du materiel au sein des etablissement</t>
+  </si>
+  <si>
+    <t>Raquage des baies</t>
   </si>
 </sst>
 </file>
@@ -902,6 +923,21 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -991,21 +1027,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="33">
@@ -1386,10 +1407,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J35"/>
+  <dimension ref="B1:N41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,23 +1456,23 @@
         <v>23</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="71" t="s">
+      <c r="D5" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="73"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="78"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="76"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="81"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="2:10" ht="7.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1497,23 +1518,23 @@
         <v>26</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="77" t="s">
+      <c r="D10" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="79"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="84"/>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="2:10" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="82"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="87"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1551,19 +1572,19 @@
         <v>44</v>
       </c>
       <c r="C15" s="58"/>
-      <c r="D15" s="105" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="105" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="105" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="105" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="105" t="s">
+      <c r="D15" s="75" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="75" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="75" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="75" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="75" t="s">
         <v>38</v>
       </c>
       <c r="J15" s="3"/>
@@ -1582,14 +1603,14 @@
       <c r="F16" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="103" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="104" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="74" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="46" t="s">
         <v>42</v>
       </c>
@@ -1610,7 +1631,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="46" t="s">
         <v>43</v>
       </c>
@@ -1631,7 +1652,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="59" t="s">
         <v>45</v>
       </c>
@@ -1652,7 +1673,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="47" t="s">
         <v>39</v>
       </c>
@@ -1673,7 +1694,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="47" t="s">
         <v>48</v>
       </c>
@@ -1694,7 +1715,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="47" t="s">
         <v>46</v>
       </c>
@@ -1715,7 +1736,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="47" t="s">
         <v>47</v>
       </c>
@@ -1736,7 +1757,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="59" t="s">
         <v>49</v>
       </c>
@@ -1757,7 +1778,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="46" t="s">
         <v>32</v>
       </c>
@@ -1778,189 +1799,318 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="47" t="s">
+    <row r="26" spans="2:14" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="47" t="s">
+      <c r="C28" s="6"/>
+      <c r="D28" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="G27" s="55" t="s">
-        <v>34</v>
-      </c>
-      <c r="H27" s="56" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="59" t="s">
+      <c r="C30" s="6"/>
+      <c r="D30" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30" s="56" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="59" t="s">
         <v>51</v>
-      </c>
-      <c r="C28" s="60"/>
-      <c r="D28" s="67" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" s="68" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" s="69" t="s">
-        <v>35</v>
-      </c>
-      <c r="G28" s="69" t="s">
-        <v>34</v>
-      </c>
-      <c r="H28" s="70" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="29"/>
-      <c r="D29" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="F29" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="G29" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="H29" s="33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="G30" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="H30" s="54" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="59" t="s">
-        <v>54</v>
       </c>
       <c r="C31" s="60"/>
       <c r="D31" s="67" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" s="69" t="s">
-        <v>35</v>
-      </c>
-      <c r="F31" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="G31" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="68" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="69" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" s="69" t="s">
         <v>34</v>
       </c>
       <c r="H31" s="70" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="46" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C32" s="29"/>
       <c r="D32" s="42" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E32" s="45" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F32" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="G32" s="102" t="s">
-        <v>34</v>
-      </c>
-      <c r="H32" s="101" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G32" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="46" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C33" s="29"/>
       <c r="D33" s="42" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E33" s="45" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F33" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="G33" s="102" t="s">
-        <v>34</v>
-      </c>
-      <c r="H33" s="101" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D35" s="83" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" s="33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="29"/>
+      <c r="D34" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="G34" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34" s="33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="29"/>
+      <c r="D35" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H35" s="33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="G36" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="H36" s="54" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="60"/>
+      <c r="D37" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="69" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="G37" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="H37" s="70" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="29"/>
+      <c r="D38" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="G38" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="H38" s="71" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="29"/>
+      <c r="D39" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="G39" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="H39" s="71" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="E35" s="84"/>
-      <c r="F35" s="84"/>
-      <c r="G35" s="84"/>
-      <c r="H35" s="85"/>
+      <c r="E41" s="89"/>
+      <c r="F41" s="89"/>
+      <c r="G41" s="89"/>
+      <c r="H41" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D5:H6"/>
     <mergeCell ref="D10:H11"/>
-    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="D41:H41"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2022,23 +2172,23 @@
         <v>9</v>
       </c>
       <c r="C5" s="13"/>
-      <c r="D5" s="89" t="s">
+      <c r="D5" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="91"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="96"/>
       <c r="I5" s="13"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="94"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="98"/>
+      <c r="H6" s="99"/>
       <c r="I6" s="13"/>
     </row>
     <row r="7" spans="2:9" ht="7.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2084,23 +2234,23 @@
         <v>14</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="95" t="s">
+      <c r="D10" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="96"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="96"/>
-      <c r="H10" s="97"/>
+      <c r="E10" s="101"/>
+      <c r="F10" s="101"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="102"/>
       <c r="I10" s="13"/>
     </row>
     <row r="11" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
-      <c r="D11" s="98"/>
-      <c r="E11" s="99"/>
-      <c r="F11" s="99"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="100"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="104"/>
+      <c r="F11" s="104"/>
+      <c r="G11" s="104"/>
+      <c r="H11" s="105"/>
       <c r="I11" s="13"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -2198,13 +2348,13 @@
     </row>
     <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="86" t="s">
+      <c r="D22" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="88"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="92"/>
+      <c r="H22" s="93"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H24" s="10" t="s">

</xml_diff>